<commit_message>
address feedback, stocksplits also for ISIN, slight wiggle room for FOREX transactions, handle nan/0 fees for schwab transactions
</commit_message>
<xml_diff>
--- a/example/stock_splits.xlsx
+++ b/example/stock_splits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/pyFIFOtax/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/pyFIFOtax/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{098EEEC9-65F1-9147-A7BB-F1E1BA3C3C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7FD725-F2C5-8449-8D48-F3F99479C0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16640" xr2:uid="{2749B324-D211-0348-BDFB-DE13BA88D932}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{2749B324-D211-0348-BDFB-DE13BA88D932}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>date</t>
   </si>
@@ -49,6 +49,9 @@
   <si>
     <t>NVDA</t>
   </si>
+  <si>
+    <t>US67066G1040</t>
+  </si>
 </sst>
 </file>
 
@@ -57,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +78,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -99,11 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,11 +448,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0153BE41-03F1-6B43-A972-5862EE571DD9}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -523,6 +531,72 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>45450</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>44397</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>39336</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>38814</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>37146</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>36704</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>